<commit_message>
Debbuged the API test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Sacred_Analytics.xlsx
+++ b/src/main/resources/Sacred_Analytics.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\IdeaProjects\untitled6\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\untitled6\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D8BB9C-A11A-4315-AA4F-5EFE176EC342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8538A0-79C7-4AD5-95FF-A34C8820F161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="408" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1992" yWindow="348" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="postReq" sheetId="1" r:id="rId1"/>
     <sheet name="TotalClustersGuard" sheetId="2" r:id="rId2"/>
+    <sheet name="postLogin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
   <si>
     <t>API Name</t>
   </si>
@@ -221,6 +222,60 @@
   </si>
   <si>
     <t>"0067e96f-2f47-4d8f-864a-0906d54173ad","e637f040-5b32-460f-86c5-1f8a594d7adc"</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Expected Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>SacredGroves@FT!@#007</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>empty string userid</t>
+  </si>
+  <si>
+    <t>empty string password</t>
+  </si>
+  <si>
+    <t>Incorrect123 @#$</t>
+  </si>
+  <si>
+    <t>Incorrect password</t>
+  </si>
+  <si>
+    <t>Adm in</t>
+  </si>
+  <si>
+    <t>space in user_id</t>
+  </si>
+  <si>
+    <t>Ad*min</t>
+  </si>
+  <si>
+    <t>Special chars in userid</t>
+  </si>
+  <si>
+    <t>@#$%^&amp;*()&gt;&lt;?.',;</t>
+  </si>
+  <si>
+    <t>blank user id</t>
+  </si>
+  <si>
+    <t>blank password</t>
   </si>
 </sst>
 </file>
@@ -913,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D5F2E6-ED0C-4707-83F8-70434EB226AF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -942,4 +997,147 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA257329-6B36-452B-A8DC-8891B9B7C49C}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>